<commit_message>
TASK-0002: change amount of sectors
</commit_message>
<xml_diff>
--- a/mathExample.xlsx
+++ b/mathExample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maksymv/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FAE1F7C-2BB3-4F40-B131-509D59EC8DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E109DFD6-3DC1-A045-AE4A-C4BBCCBC3C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{6A40DD33-E6B5-FF46-B381-B951678C493F}"/>
   </bookViews>
@@ -482,7 +482,7 @@
   <dimension ref="B4:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,7 +507,7 @@
       </c>
       <c r="D5" s="5">
         <f>C5/C$11</f>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
@@ -515,11 +515,11 @@
         <v>20</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D6" s="5">
         <f t="shared" ref="D6:D10" si="0">C6/C$11</f>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
@@ -531,7 +531,7 @@
       </c>
       <c r="D7" s="5">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
@@ -539,11 +539,11 @@
         <v>27</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D8" s="5">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
@@ -555,7 +555,7 @@
       </c>
       <c r="D9" s="5">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
@@ -567,17 +567,17 @@
       </c>
       <c r="D10" s="5">
         <f t="shared" si="0"/>
-        <v>0.16666666666666666</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C11">
         <f>SUM(C5:C10)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D11">
         <f>SUM(D5:D10)</f>
-        <v>0.99999999999999989</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
@@ -586,7 +586,7 @@
       </c>
       <c r="C13">
         <f>SUMPRODUCT(B5:B10,D5:D10)</f>
-        <v>26.166666666666664</v>
+        <v>25.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>